<commit_message>
Row validation for incomplete data.
</commit_message>
<xml_diff>
--- a/database/seeds/csvs/camps.xlsx
+++ b/database/seeds/csvs/camps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Poom\ICT\Senior\campass\database\seeds\csvs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE6D7E0-0A1A-4B49-88AB-CB3F253F5496}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C89ECF-054A-440B-AFAF-A02E8C168C68}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8DF051AC-2325-4821-AF8F-205C9028BC53}"/>
   </bookViews>
@@ -1025,7 +1025,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="yyyy\-m\-d\ h:m:s"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-m\-d\ h:m:s"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -1126,7 +1126,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1134,22 +1134,22 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy\-m\-d\ h:m:s"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-m\-d\ h:m:s"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy\-m\-d\ h:m:s"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-m\-d\ h:m:s"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy\-m\-d\ h:m:s"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-m\-d\ h:m:s"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy\-m\-d\ h:m:s"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-m\-d\ h:m:s"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy\-m\-d\ h:m:s"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-m\-d\ h:m:s"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy\-m\-d\ h:m:s"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-m\-d\ h:m:s"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -1513,8 +1513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{324C8412-2BD7-48F7-B020-E53CBC6718C3}">
   <dimension ref="A1:AD52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1:Y1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>